<commit_message>
Minor corrections to 5 scripts
</commit_message>
<xml_diff>
--- a/tl/S10021.MES.BIN.xlsx
+++ b/tl/S10021.MES.BIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486FF4D9-60FF-455A-96FB-B64BC1C17DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53FF69B-660B-4D05-BC69-C2012AAA4328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="5070" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="16215" windowWidth="55245" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S10021.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>Click.</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -129,13 +126,16 @@
   </si>
   <si>
     <t>…I was incredibly happy, and at the same time, felt a little bit lonely.</t>
+  </si>
+  <si>
+    <t>Plop.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -550,9 +550,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
@@ -560,7 +562,7 @@
     <col min="5" max="10" width="115" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -612,391 +614,391 @@
         <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>9</v>

</xml_diff>